<commit_message>
system test - coverd tc id
</commit_message>
<xml_diff>
--- a/defect_category_2.xlsx
+++ b/defect_category_2.xlsx
@@ -23,13 +23,13 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Code Review'!$B$3:$I$113</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">통합!$A$1:$M$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">통합!$A$1:$AI$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId9"/>
-    <pivotCache cacheId="13" r:id="rId10"/>
-    <pivotCache cacheId="14" r:id="rId11"/>
+    <pivotCache cacheId="15" r:id="rId9"/>
+    <pivotCache cacheId="16" r:id="rId10"/>
+    <pivotCache cacheId="17" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2844" uniqueCount="468">
   <si>
     <t>SonarQube</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1336,6 +1336,172 @@
   </si>
   <si>
     <t>[Defect] save/load : rooms visit information error.  - at load time, current room is in room visited.</t>
+  </si>
+  <si>
+    <t>tc_p25</t>
+  </si>
+  <si>
+    <t>tc_p20</t>
+  </si>
+  <si>
+    <t>tc_p8</t>
+  </si>
+  <si>
+    <t>tc_p22, tc_p24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_p24</t>
+  </si>
+  <si>
+    <t>tc_p22</t>
+  </si>
+  <si>
+    <t>tc_opensafe</t>
+  </si>
+  <si>
+    <t>tc_cr21</t>
+  </si>
+  <si>
+    <t>tc_cr18</t>
+  </si>
+  <si>
+    <t>tc_cr11</t>
+  </si>
+  <si>
+    <t>tc_cr12, tc_cr13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_cr16</t>
+  </si>
+  <si>
+    <t>tc_cr7</t>
+  </si>
+  <si>
+    <t>tc_cr06</t>
+  </si>
+  <si>
+    <t>tc_cg3</t>
+  </si>
+  <si>
+    <t>tc_cg6</t>
+  </si>
+  <si>
+    <t>tc_cg5</t>
+  </si>
+  <si>
+    <t>tc_cr4</t>
+  </si>
+  <si>
+    <t>tc_cr22</t>
+  </si>
+  <si>
+    <t>tc_detonatedynamite</t>
+  </si>
+  <si>
+    <t>tc_cr19</t>
+  </si>
+  <si>
+    <t>tc_startmicrowave</t>
+  </si>
+  <si>
+    <t>tc_p26</t>
+  </si>
+  <si>
+    <t>tc_openlock</t>
+  </si>
+  <si>
+    <t>tc_enter, tc_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_uc04</t>
+  </si>
+  <si>
+    <t>tc_p1</t>
+  </si>
+  <si>
+    <t>tc_e4</t>
+  </si>
+  <si>
+    <t>tc_p12</t>
+  </si>
+  <si>
+    <t>tc_p2, tc_removedocumentinsafe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_putgoldinlock</t>
+  </si>
+  <si>
+    <t>tc_removedocumentinsafe</t>
+  </si>
+  <si>
+    <t>tc_eatcoffee, tc_eatfood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_digshovel</t>
+  </si>
+  <si>
+    <t>tc_removegoldinpot</t>
+  </si>
+  <si>
+    <t>tc_openlock, tc_putkeyinlock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_breakpot</t>
+  </si>
+  <si>
+    <t>tc_p4, tc_p5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_p9, tc_digshovel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_allaction</t>
+  </si>
+  <si>
+    <t>tc_inspectaction</t>
+  </si>
+  <si>
+    <t>tc_installaction, tc_putaction, tc_removeaction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tc_uc06</t>
+  </si>
+  <si>
+    <t>tc_uc10</t>
+  </si>
+  <si>
+    <t>tc_uc09</t>
+  </si>
+  <si>
+    <t>tc_p6</t>
+  </si>
+  <si>
+    <t>tc_p3</t>
+  </si>
+  <si>
+    <t>tc_picupkey</t>
+  </si>
+  <si>
+    <t>tc_uc03</t>
+  </si>
+  <si>
+    <t>tc_p5</t>
+  </si>
+  <si>
+    <t>tc_uc02</t>
+  </si>
+  <si>
+    <t>covered TC ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1510,7 +1676,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1576,6 +1742,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1698,7 +1867,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1756,11 +1924,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="388866056"/>
-        <c:axId val="388866448"/>
+        <c:axId val="328403016"/>
+        <c:axId val="328403408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="388866056"/>
+        <c:axId val="328403016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,7 +1971,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388866448"/>
+        <c:crossAx val="328403408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1811,7 +1979,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="388866448"/>
+        <c:axId val="328403408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,7 +2030,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388866056"/>
+        <c:crossAx val="328403016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2001,11 +2169,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="442611848"/>
-        <c:axId val="442612240"/>
+        <c:axId val="328404192"/>
+        <c:axId val="328404584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="442611848"/>
+        <c:axId val="328404192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2048,7 +2216,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442612240"/>
+        <c:crossAx val="328404584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2056,7 +2224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442612240"/>
+        <c:axId val="328404584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2107,7 +2275,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442611848"/>
+        <c:crossAx val="328404192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2459,11 +2627,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="442613024"/>
-        <c:axId val="442613416"/>
+        <c:axId val="271098352"/>
+        <c:axId val="271098744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="442613024"/>
+        <c:axId val="271098352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2506,7 +2674,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442613416"/>
+        <c:crossAx val="271098744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2514,7 +2682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442613416"/>
+        <c:axId val="271098744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,7 +2733,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442613024"/>
+        <c:crossAx val="271098352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3286,11 +3454,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="442614200"/>
-        <c:axId val="442614592"/>
+        <c:axId val="271099528"/>
+        <c:axId val="271099920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="442614200"/>
+        <c:axId val="271099528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3333,7 +3501,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442614592"/>
+        <c:crossAx val="271099920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3341,7 +3509,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442614592"/>
+        <c:axId val="271099920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3392,7 +3560,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442614200"/>
+        <c:crossAx val="271099528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3573,11 +3741,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="440318040"/>
-        <c:axId val="440318432"/>
+        <c:axId val="271100704"/>
+        <c:axId val="271101096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="440318040"/>
+        <c:axId val="271100704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3620,7 +3788,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440318432"/>
+        <c:crossAx val="271101096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3628,7 +3796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="440318432"/>
+        <c:axId val="271101096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3679,7 +3847,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440318040"/>
+        <c:crossAx val="271100704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3823,7 +3991,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3882,11 +4049,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="440319216"/>
-        <c:axId val="440319608"/>
+        <c:axId val="399109104"/>
+        <c:axId val="399109496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="440319216"/>
+        <c:axId val="399109104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3929,7 +4096,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440319608"/>
+        <c:crossAx val="399109496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3937,7 +4104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="440319608"/>
+        <c:axId val="399109496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3988,7 +4155,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440319216"/>
+        <c:crossAx val="399109104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9480,7 +9647,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -9529,7 +9696,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블2" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -9612,7 +9779,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블11" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블11" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -9669,7 +9836,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="피벗 테이블1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -10554,10 +10721,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M209"/>
+  <dimension ref="A1:AI209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N70" sqref="N70:N72"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10575,7 +10742,7 @@
     <col min="12" max="12" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>148</v>
       </c>
@@ -10615,8 +10782,11 @@
       <c r="M1" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -10647,8 +10817,11 @@
       <c r="K2" s="4">
         <v>43313.69027777778</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -10679,8 +10852,11 @@
       <c r="K3" s="4">
         <v>43313.69027777778</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -10714,8 +10890,11 @@
       <c r="K4" s="4">
         <v>43309.468055555553</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -10746,8 +10925,11 @@
       <c r="K5" s="4">
         <v>43313.689583333333</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>158</v>
       </c>
@@ -10781,8 +10963,11 @@
       <c r="K6" s="4">
         <v>43313.689583333333</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -10816,9 +11001,12 @@
       <c r="K7" s="4">
         <v>43313.689583333333</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="N7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B8" t="s">
@@ -10827,7 +11015,7 @@
       <c r="C8">
         <v>10113</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="21" t="s">
         <v>348</v>
       </c>
       <c r="E8" t="s">
@@ -10836,7 +11024,7 @@
       <c r="F8" t="s">
         <v>315</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H8" t="s">
@@ -10852,8 +11040,8 @@
         <v>43313.536805555559</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B9" t="s">
@@ -10862,7 +11050,7 @@
       <c r="C9">
         <v>10114</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="21" t="s">
         <v>346</v>
       </c>
       <c r="E9" t="s">
@@ -10871,7 +11059,7 @@
       <c r="F9" t="s">
         <v>315</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H9" t="s">
@@ -10887,8 +11075,8 @@
         <v>43313.536805555559</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B10" t="s">
@@ -10897,7 +11085,7 @@
       <c r="C10">
         <v>10115</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="21" t="s">
         <v>344</v>
       </c>
       <c r="E10" t="s">
@@ -10906,7 +11094,7 @@
       <c r="F10" t="s">
         <v>315</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="21" t="s">
         <v>374</v>
       </c>
       <c r="H10" t="s">
@@ -10922,8 +11110,8 @@
         <v>43313.536805555559</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B11" t="s">
@@ -10932,7 +11120,7 @@
       <c r="C11">
         <v>10116</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="21" t="s">
         <v>342</v>
       </c>
       <c r="E11" t="s">
@@ -10941,7 +11129,7 @@
       <c r="F11" t="s">
         <v>315</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="21" t="s">
         <v>374</v>
       </c>
       <c r="H11" t="s">
@@ -10957,8 +11145,8 @@
         <v>43313.536805555559</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B12" t="s">
@@ -10967,7 +11155,7 @@
       <c r="C12">
         <v>10119</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="21" t="s">
         <v>340</v>
       </c>
       <c r="E12" t="s">
@@ -10976,7 +11164,7 @@
       <c r="F12" t="s">
         <v>315</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="21" t="s">
         <v>374</v>
       </c>
       <c r="H12" t="s">
@@ -10992,7 +11180,7 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>158</v>
       </c>
@@ -11023,8 +11211,11 @@
       <c r="K13" s="4">
         <v>43313.689583333333</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -11055,8 +11246,11 @@
       <c r="K14" s="4">
         <v>43313.689583333333</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>158</v>
       </c>
@@ -11090,9 +11284,12 @@
       <c r="K15" s="4">
         <v>43309.468055555553</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="N15" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B16" t="s">
@@ -11101,7 +11298,7 @@
       <c r="C16">
         <v>10124</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="21" t="s">
         <v>332</v>
       </c>
       <c r="E16" t="s">
@@ -11110,7 +11307,7 @@
       <c r="F16" t="s">
         <v>315</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H16" t="s">
@@ -11126,8 +11323,8 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B17" t="s">
@@ -11136,7 +11333,7 @@
       <c r="C17">
         <v>10125</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="21" t="s">
         <v>330</v>
       </c>
       <c r="E17" t="s">
@@ -11145,7 +11342,7 @@
       <c r="F17" t="s">
         <v>315</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H17" t="s">
@@ -11161,8 +11358,8 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B18" t="s">
@@ -11171,7 +11368,7 @@
       <c r="C18">
         <v>10126</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="21" t="s">
         <v>328</v>
       </c>
       <c r="E18" t="s">
@@ -11180,7 +11377,7 @@
       <c r="F18" t="s">
         <v>315</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H18" t="s">
@@ -11196,8 +11393,8 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B19" t="s">
@@ -11206,7 +11403,7 @@
       <c r="C19">
         <v>10128</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="21" t="s">
         <v>326</v>
       </c>
       <c r="E19" t="s">
@@ -11215,7 +11412,7 @@
       <c r="F19" t="s">
         <v>315</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H19" t="s">
@@ -11231,8 +11428,8 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B20" t="s">
@@ -11241,7 +11438,7 @@
       <c r="C20">
         <v>10129</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="21" t="s">
         <v>324</v>
       </c>
       <c r="E20" t="s">
@@ -11250,7 +11447,7 @@
       <c r="F20" t="s">
         <v>315</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H20" t="s">
@@ -11266,8 +11463,8 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B21" t="s">
@@ -11276,7 +11473,7 @@
       <c r="C21">
         <v>10130</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="21" t="s">
         <v>322</v>
       </c>
       <c r="E21" t="s">
@@ -11285,7 +11482,7 @@
       <c r="F21" t="s">
         <v>315</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H21" t="s">
@@ -11301,8 +11498,8 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B22" t="s">
@@ -11311,7 +11508,7 @@
       <c r="C22">
         <v>10131</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="21" t="s">
         <v>320</v>
       </c>
       <c r="E22" t="s">
@@ -11320,7 +11517,7 @@
       <c r="F22" t="s">
         <v>315</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H22" t="s">
@@ -11336,8 +11533,8 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B23" t="s">
@@ -11346,7 +11543,7 @@
       <c r="C23">
         <v>10132</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="21" t="s">
         <v>318</v>
       </c>
       <c r="E23" t="s">
@@ -11355,7 +11552,7 @@
       <c r="F23" t="s">
         <v>315</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H23" t="s">
@@ -11371,8 +11568,8 @@
         <v>43313.579861111109</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B24" t="s">
@@ -11381,7 +11578,7 @@
       <c r="C24">
         <v>10133</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="21" t="s">
         <v>314</v>
       </c>
       <c r="E24" t="s">
@@ -11390,7 +11587,7 @@
       <c r="F24" t="s">
         <v>315</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H24" t="s">
@@ -11406,7 +11603,7 @@
         <v>43313.578472222223</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>158</v>
       </c>
@@ -11440,8 +11637,11 @@
       <c r="K25" s="4">
         <v>43309.46875</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>158</v>
       </c>
@@ -11475,8 +11675,11 @@
       <c r="K26" s="4">
         <v>43313.688888888886</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N26" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>158</v>
       </c>
@@ -11510,8 +11713,11 @@
       <c r="K27" s="4">
         <v>43309.474999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>158</v>
       </c>
@@ -11545,8 +11751,11 @@
       <c r="K28" s="4">
         <v>43309.474999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>158</v>
       </c>
@@ -11580,8 +11789,11 @@
       <c r="K29" s="4">
         <v>43309.474999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N29" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>158</v>
       </c>
@@ -11615,8 +11827,11 @@
       <c r="K30" s="4">
         <v>43309.475694444445</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N30" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>158</v>
       </c>
@@ -11647,8 +11862,11 @@
       <c r="K31" s="4">
         <v>43309.680555555555</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N31" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>158</v>
       </c>
@@ -11679,9 +11897,12 @@
       <c r="K32" s="4">
         <v>43313.467361111114</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="N32" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B33" t="s">
@@ -11690,7 +11911,7 @@
       <c r="C33">
         <v>10153</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="21" t="s">
         <v>296</v>
       </c>
       <c r="E33" t="s">
@@ -11699,10 +11920,10 @@
       <c r="F33" t="s">
         <v>168</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="21" t="s">
         <v>161</v>
       </c>
       <c r="I33" t="s">
@@ -11715,7 +11936,7 @@
         <v>43311.59375</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -11749,8 +11970,11 @@
       <c r="K34" s="4">
         <v>43310.92291666667</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N34" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>158</v>
       </c>
@@ -11785,7 +12009,7 @@
         <v>43311.411111111112</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -11820,7 +12044,7 @@
         <v>43311.411111111112</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>158</v>
       </c>
@@ -11855,7 +12079,7 @@
         <v>43311.411111111112</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>158</v>
       </c>
@@ -11889,8 +12113,11 @@
       <c r="K38" s="4">
         <v>43311.916666666664</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N38" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>158</v>
       </c>
@@ -11924,9 +12151,12 @@
       <c r="K39" s="4">
         <v>43313.6875</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="N39" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B40" t="s">
@@ -11935,7 +12165,7 @@
       <c r="C40">
         <v>10161</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="21" t="s">
         <v>281</v>
       </c>
       <c r="E40" t="s">
@@ -11944,7 +12174,7 @@
       <c r="F40" t="s">
         <v>136</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H40" t="s">
@@ -11960,8 +12190,8 @@
         <v>43311.472222222219</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B41" t="s">
@@ -11970,7 +12200,7 @@
       <c r="C41">
         <v>10162</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="21" t="s">
         <v>279</v>
       </c>
       <c r="E41" t="s">
@@ -11979,7 +12209,7 @@
       <c r="F41" t="s">
         <v>136</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="21" t="s">
         <v>373</v>
       </c>
       <c r="H41" t="s">
@@ -11995,8 +12225,8 @@
         <v>43311.472222222219</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B42" t="s">
@@ -12005,7 +12235,7 @@
       <c r="C42">
         <v>10164</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="21" t="s">
         <v>277</v>
       </c>
       <c r="E42" t="s">
@@ -12014,7 +12244,7 @@
       <c r="F42" t="s">
         <v>168</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="21" t="s">
         <v>374</v>
       </c>
       <c r="H42" t="s">
@@ -12030,8 +12260,8 @@
         <v>43311.474999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B43" t="s">
@@ -12040,7 +12270,7 @@
       <c r="C43">
         <v>10165</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="21" t="s">
         <v>275</v>
       </c>
       <c r="E43" t="s">
@@ -12049,7 +12279,7 @@
       <c r="F43" t="s">
         <v>168</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="21" t="s">
         <v>374</v>
       </c>
       <c r="H43" t="s">
@@ -12065,8 +12295,8 @@
         <v>43311.658333333333</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B44" t="s">
@@ -12075,7 +12305,7 @@
       <c r="C44">
         <v>10166</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="21" t="s">
         <v>273</v>
       </c>
       <c r="E44" t="s">
@@ -12084,7 +12314,7 @@
       <c r="F44" t="s">
         <v>168</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="21" t="s">
         <v>374</v>
       </c>
       <c r="H44" t="s">
@@ -12100,7 +12330,7 @@
         <v>43313.449305555558</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>158</v>
       </c>
@@ -12134,8 +12364,11 @@
       <c r="K45" s="4">
         <v>43313.686805555553</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N45" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>158</v>
       </c>
@@ -12169,8 +12402,11 @@
       <c r="K46" s="4">
         <v>43313.686111111114</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N46" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>158</v>
       </c>
@@ -12201,8 +12437,11 @@
       <c r="K47" s="4">
         <v>43313.686111111114</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N47" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>158</v>
       </c>
@@ -12236,8 +12475,11 @@
       <c r="K48" s="4">
         <v>43313.685416666667</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N48" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>158</v>
       </c>
@@ -12271,8 +12513,11 @@
       <c r="K49" s="4">
         <v>43313.685416666667</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N49" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>158</v>
       </c>
@@ -12306,8 +12551,11 @@
       <c r="K50" s="4">
         <v>43313.542361111111</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N50" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>158</v>
       </c>
@@ -12338,8 +12586,11 @@
       <c r="K51" s="4">
         <v>43313.544444444444</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N51" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>158</v>
       </c>
@@ -12370,8 +12621,11 @@
       <c r="K52" s="4">
         <v>43313.488888888889</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N52" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>158</v>
       </c>
@@ -12402,8 +12656,11 @@
       <c r="K53" s="4">
         <v>43313.545138888891</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N53" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>158</v>
       </c>
@@ -12434,8 +12691,11 @@
       <c r="K54" s="4">
         <v>43313.365277777775</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N54" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>158</v>
       </c>
@@ -12466,8 +12726,11 @@
       <c r="K55" s="4">
         <v>43313.368055555555</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N55" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>158</v>
       </c>
@@ -12498,8 +12761,11 @@
       <c r="K56" s="4">
         <v>43313.371527777781</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N56" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>158</v>
       </c>
@@ -12533,8 +12799,11 @@
       <c r="K57" s="4">
         <v>43309.459027777775</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N57" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>158</v>
       </c>
@@ -12565,8 +12834,11 @@
       <c r="K58" s="4">
         <v>43313.373611111114</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N58" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>158</v>
       </c>
@@ -12597,8 +12869,11 @@
       <c r="K59" s="4">
         <v>43313.46875</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N59" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>158</v>
       </c>
@@ -12629,8 +12904,11 @@
       <c r="K60" s="4">
         <v>43313.46875</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N60" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>158</v>
       </c>
@@ -12661,8 +12939,11 @@
       <c r="K61" s="4">
         <v>43313.46875</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N61" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>158</v>
       </c>
@@ -12693,8 +12974,11 @@
       <c r="K62" s="4">
         <v>43313.68472222222</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N62" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>158</v>
       </c>
@@ -12728,9 +13012,12 @@
       <c r="K63" s="4">
         <v>43313.684027777781</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="N63" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A64" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B64" t="s">
@@ -12739,7 +13026,7 @@
       <c r="C64">
         <v>10195</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="21" t="s">
         <v>235</v>
       </c>
       <c r="E64" t="s">
@@ -12748,7 +13035,7 @@
       <c r="F64" t="s">
         <v>168</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" s="21" t="s">
         <v>374</v>
       </c>
       <c r="H64" t="s">
@@ -12764,7 +13051,7 @@
         <v>43313.53402777778</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>158</v>
       </c>
@@ -12795,8 +13082,11 @@
       <c r="K65" s="4">
         <v>43313.628472222219</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N65" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>158</v>
       </c>
@@ -12830,8 +13120,11 @@
       <c r="K66" s="4">
         <v>43313.68472222222</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N66" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>158</v>
       </c>
@@ -12862,8 +13155,11 @@
       <c r="K67" s="4">
         <v>43313.68472222222</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N67" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>158</v>
       </c>
@@ -12897,8 +13193,11 @@
       <c r="K68" s="4">
         <v>43313.692361111112</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N68" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>158</v>
       </c>
@@ -12932,8 +13231,11 @@
       <c r="K69" s="4">
         <v>43313.68472222222</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N69" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="22" t="s">
         <v>158</v>
       </c>
@@ -12964,8 +13266,11 @@
       <c r="K70" s="4">
         <v>43313.8</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N70" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="22" t="s">
         <v>158</v>
       </c>
@@ -12996,8 +13301,11 @@
       <c r="K71" s="4">
         <v>43313.820138888892</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N71" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="22" t="s">
         <v>158</v>
       </c>
@@ -13028,8 +13336,11 @@
       <c r="K72" s="4">
         <v>43313.831250000003</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N72" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>158</v>
       </c>
@@ -13063,8 +13374,11 @@
       <c r="K73" s="4">
         <v>43309.455555555556</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N73" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>158</v>
       </c>
@@ -13098,8 +13412,11 @@
       <c r="K74" s="4">
         <v>43309.456944444442</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N74" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>158</v>
       </c>
@@ -13133,8 +13450,11 @@
       <c r="K75" s="4">
         <v>43313.692361111112</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N75" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>158</v>
       </c>
@@ -13168,8 +13488,11 @@
       <c r="K76" s="4">
         <v>43309.459722222222</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N76" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>158</v>
       </c>
@@ -13203,8 +13526,11 @@
       <c r="K77" s="4">
         <v>43309.460416666669</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N77" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>158</v>
       </c>
@@ -13238,8 +13564,11 @@
       <c r="K78" s="4">
         <v>43313.691666666666</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N78" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>158</v>
       </c>
@@ -13273,8 +13602,11 @@
       <c r="K79" s="4">
         <v>43313.691666666666</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N79" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -13308,8 +13640,11 @@
       <c r="K80" s="4">
         <v>43313.691666666666</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N80" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -13343,8 +13678,11 @@
       <c r="K81" s="4">
         <v>43313.691666666666</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N81" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>158</v>
       </c>
@@ -13378,8 +13716,11 @@
       <c r="K82" s="4">
         <v>43309.694444444445</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N82" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>158</v>
       </c>
@@ -13413,8 +13754,33 @@
       <c r="K83" s="4">
         <v>43309.46597222222</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M83" s="23"/>
+      <c r="N83" t="s">
+        <v>461</v>
+      </c>
+      <c r="O83" s="23"/>
+      <c r="P83" s="23"/>
+      <c r="Q83" s="23"/>
+      <c r="R83" s="23"/>
+      <c r="S83" s="23"/>
+      <c r="T83" s="23"/>
+      <c r="U83" s="23"/>
+      <c r="V83" s="23"/>
+      <c r="W83" s="23"/>
+      <c r="X83" s="23"/>
+      <c r="Y83" s="23"/>
+      <c r="Z83" s="23"/>
+      <c r="AA83" s="23"/>
+      <c r="AB83" s="23"/>
+      <c r="AC83" s="23"/>
+      <c r="AD83" s="23"/>
+      <c r="AE83" s="23"/>
+      <c r="AF83" s="23"/>
+      <c r="AG83" s="23"/>
+      <c r="AH83" s="23"/>
+      <c r="AI83" s="23"/>
+    </row>
+    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>158</v>
       </c>
@@ -13448,8 +13814,33 @@
       <c r="K84" s="4">
         <v>43309.466666666667</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M84" s="23"/>
+      <c r="N84" t="s">
+        <v>462</v>
+      </c>
+      <c r="O84" s="23"/>
+      <c r="P84" s="23"/>
+      <c r="Q84" s="23"/>
+      <c r="R84" s="23"/>
+      <c r="S84" s="23"/>
+      <c r="T84" s="23"/>
+      <c r="U84" s="23"/>
+      <c r="V84" s="23"/>
+      <c r="W84" s="23"/>
+      <c r="X84" s="23"/>
+      <c r="Y84" s="23"/>
+      <c r="Z84" s="23"/>
+      <c r="AA84" s="23"/>
+      <c r="AB84" s="23"/>
+      <c r="AC84" s="23"/>
+      <c r="AD84" s="23"/>
+      <c r="AE84" s="23"/>
+      <c r="AF84" s="23"/>
+      <c r="AG84" s="23"/>
+      <c r="AH84" s="23"/>
+      <c r="AI84" s="23"/>
+    </row>
+    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>158</v>
       </c>
@@ -13483,8 +13874,33 @@
       <c r="K85" s="4">
         <v>43309.664583333331</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M85" s="23"/>
+      <c r="N85" t="s">
+        <v>422</v>
+      </c>
+      <c r="O85" s="23"/>
+      <c r="P85" s="23"/>
+      <c r="Q85" s="23"/>
+      <c r="R85" s="23"/>
+      <c r="S85" s="23"/>
+      <c r="T85" s="23"/>
+      <c r="U85" s="23"/>
+      <c r="V85" s="23"/>
+      <c r="W85" s="23"/>
+      <c r="X85" s="23"/>
+      <c r="Y85" s="23"/>
+      <c r="Z85" s="23"/>
+      <c r="AA85" s="23"/>
+      <c r="AB85" s="23"/>
+      <c r="AC85" s="23"/>
+      <c r="AD85" s="23"/>
+      <c r="AE85" s="23"/>
+      <c r="AF85" s="23"/>
+      <c r="AG85" s="23"/>
+      <c r="AH85" s="23"/>
+      <c r="AI85" s="23"/>
+    </row>
+    <row r="86" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -13519,10 +13935,34 @@
         <v>43309.466666666667</v>
       </c>
       <c r="L86"/>
-      <c r="M86"/>
-    </row>
-    <row r="87" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="M86" s="23"/>
+      <c r="N86" t="s">
+        <v>463</v>
+      </c>
+      <c r="O86" s="23"/>
+      <c r="P86" s="23"/>
+      <c r="Q86" s="23"/>
+      <c r="R86" s="23"/>
+      <c r="S86" s="23"/>
+      <c r="T86" s="23"/>
+      <c r="U86" s="23"/>
+      <c r="V86" s="23"/>
+      <c r="W86" s="23"/>
+      <c r="X86" s="23"/>
+      <c r="Y86" s="23"/>
+      <c r="Z86" s="23"/>
+      <c r="AA86" s="23"/>
+      <c r="AB86" s="23"/>
+      <c r="AC86" s="23"/>
+      <c r="AD86" s="23"/>
+      <c r="AE86" s="23"/>
+      <c r="AF86" s="23"/>
+      <c r="AG86" s="23"/>
+      <c r="AH86" s="23"/>
+      <c r="AI86" s="23"/>
+    </row>
+    <row r="87" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B87" t="s">
@@ -13531,7 +13971,7 @@
       <c r="C87">
         <v>10045</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="21" t="s">
         <v>160</v>
       </c>
       <c r="E87" t="s">
@@ -13556,9 +13996,31 @@
         <v>43313.439583333333</v>
       </c>
       <c r="L87"/>
-      <c r="M87"/>
-    </row>
-    <row r="88" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M87" s="23"/>
+      <c r="N87" s="23"/>
+      <c r="O87" s="23"/>
+      <c r="P87" s="23"/>
+      <c r="Q87" s="23"/>
+      <c r="R87" s="23"/>
+      <c r="S87" s="23"/>
+      <c r="T87" s="23"/>
+      <c r="U87" s="23"/>
+      <c r="V87" s="23"/>
+      <c r="W87" s="23"/>
+      <c r="X87" s="23"/>
+      <c r="Y87" s="23"/>
+      <c r="Z87" s="23"/>
+      <c r="AA87" s="23"/>
+      <c r="AB87" s="23"/>
+      <c r="AC87" s="23"/>
+      <c r="AD87" s="23"/>
+      <c r="AE87" s="23"/>
+      <c r="AF87" s="23"/>
+      <c r="AG87" s="23"/>
+      <c r="AH87" s="23"/>
+      <c r="AI87" s="23"/>
+    </row>
+    <row r="88" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>158</v>
       </c>
@@ -13593,9 +14055,31 @@
         <v>43299.957638888889</v>
       </c>
       <c r="L88"/>
-      <c r="M88"/>
-    </row>
-    <row r="89" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M88" s="23"/>
+      <c r="N88" s="23"/>
+      <c r="O88" s="23"/>
+      <c r="P88" s="23"/>
+      <c r="Q88" s="23"/>
+      <c r="R88" s="23"/>
+      <c r="S88" s="23"/>
+      <c r="T88" s="23"/>
+      <c r="U88" s="23"/>
+      <c r="V88" s="23"/>
+      <c r="W88" s="23"/>
+      <c r="X88" s="23"/>
+      <c r="Y88" s="23"/>
+      <c r="Z88" s="23"/>
+      <c r="AA88" s="23"/>
+      <c r="AB88" s="23"/>
+      <c r="AC88" s="23"/>
+      <c r="AD88" s="23"/>
+      <c r="AE88" s="23"/>
+      <c r="AF88" s="23"/>
+      <c r="AG88" s="23"/>
+      <c r="AH88" s="23"/>
+      <c r="AI88" s="23"/>
+    </row>
+    <row r="89" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>158</v>
       </c>
@@ -13630,9 +14114,31 @@
         <v>43299.922222222223</v>
       </c>
       <c r="L89"/>
-      <c r="M89"/>
-    </row>
-    <row r="90" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M89" s="23"/>
+      <c r="N89" s="23"/>
+      <c r="O89" s="23"/>
+      <c r="P89" s="23"/>
+      <c r="Q89" s="23"/>
+      <c r="R89" s="23"/>
+      <c r="S89" s="23"/>
+      <c r="T89" s="23"/>
+      <c r="U89" s="23"/>
+      <c r="V89" s="23"/>
+      <c r="W89" s="23"/>
+      <c r="X89" s="23"/>
+      <c r="Y89" s="23"/>
+      <c r="Z89" s="23"/>
+      <c r="AA89" s="23"/>
+      <c r="AB89" s="23"/>
+      <c r="AC89" s="23"/>
+      <c r="AD89" s="23"/>
+      <c r="AE89" s="23"/>
+      <c r="AF89" s="23"/>
+      <c r="AG89" s="23"/>
+      <c r="AH89" s="23"/>
+      <c r="AI89" s="23"/>
+    </row>
+    <row r="90" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>158</v>
       </c>
@@ -13667,9 +14173,31 @@
         <v>43299.95208333333</v>
       </c>
       <c r="L90"/>
-      <c r="M90"/>
-    </row>
-    <row r="91" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M90" s="23"/>
+      <c r="N90" s="23"/>
+      <c r="O90" s="23"/>
+      <c r="P90" s="23"/>
+      <c r="Q90" s="23"/>
+      <c r="R90" s="23"/>
+      <c r="S90" s="23"/>
+      <c r="T90" s="23"/>
+      <c r="U90" s="23"/>
+      <c r="V90" s="23"/>
+      <c r="W90" s="23"/>
+      <c r="X90" s="23"/>
+      <c r="Y90" s="23"/>
+      <c r="Z90" s="23"/>
+      <c r="AA90" s="23"/>
+      <c r="AB90" s="23"/>
+      <c r="AC90" s="23"/>
+      <c r="AD90" s="23"/>
+      <c r="AE90" s="23"/>
+      <c r="AF90" s="23"/>
+      <c r="AG90" s="23"/>
+      <c r="AH90" s="23"/>
+      <c r="AI90" s="23"/>
+    </row>
+    <row r="91" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>158</v>
       </c>
@@ -13704,10 +14232,34 @@
         <v>43304.720833333333</v>
       </c>
       <c r="L91"/>
-      <c r="M91"/>
-    </row>
-    <row r="92" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="M91" s="23"/>
+      <c r="N91" t="s">
+        <v>464</v>
+      </c>
+      <c r="O91" s="23"/>
+      <c r="P91" s="23"/>
+      <c r="Q91" s="23"/>
+      <c r="R91" s="23"/>
+      <c r="S91" s="23"/>
+      <c r="T91" s="23"/>
+      <c r="U91" s="23"/>
+      <c r="V91" s="23"/>
+      <c r="W91" s="23"/>
+      <c r="X91" s="23"/>
+      <c r="Y91" s="23"/>
+      <c r="Z91" s="23"/>
+      <c r="AA91" s="23"/>
+      <c r="AB91" s="23"/>
+      <c r="AC91" s="23"/>
+      <c r="AD91" s="23"/>
+      <c r="AE91" s="23"/>
+      <c r="AF91" s="23"/>
+      <c r="AG91" s="23"/>
+      <c r="AH91" s="23"/>
+      <c r="AI91" s="23"/>
+    </row>
+    <row r="92" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B92" t="s">
@@ -13716,7 +14268,7 @@
       <c r="C92">
         <v>10052</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="21" t="s">
         <v>167</v>
       </c>
       <c r="E92" t="s">
@@ -13741,9 +14293,33 @@
         <v>43304.724999999999</v>
       </c>
       <c r="L92"/>
-      <c r="M92"/>
-    </row>
-    <row r="93" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M92" s="23"/>
+      <c r="N92" t="s">
+        <v>442</v>
+      </c>
+      <c r="O92" s="23"/>
+      <c r="P92" s="23"/>
+      <c r="Q92" s="23"/>
+      <c r="R92" s="23"/>
+      <c r="S92" s="23"/>
+      <c r="T92" s="23"/>
+      <c r="U92" s="23"/>
+      <c r="V92" s="23"/>
+      <c r="W92" s="23"/>
+      <c r="X92" s="23"/>
+      <c r="Y92" s="23"/>
+      <c r="Z92" s="23"/>
+      <c r="AA92" s="23"/>
+      <c r="AB92" s="23"/>
+      <c r="AC92" s="23"/>
+      <c r="AD92" s="23"/>
+      <c r="AE92" s="23"/>
+      <c r="AF92" s="23"/>
+      <c r="AG92" s="23"/>
+      <c r="AH92" s="23"/>
+      <c r="AI92" s="23"/>
+    </row>
+    <row r="93" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>158</v>
       </c>
@@ -13778,10 +14354,32 @@
         <v>43313.398611111108</v>
       </c>
       <c r="L93"/>
-      <c r="M93"/>
-    </row>
-    <row r="94" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="M93" s="23"/>
+      <c r="N93" s="23"/>
+      <c r="O93" s="23"/>
+      <c r="P93" s="23"/>
+      <c r="Q93" s="23"/>
+      <c r="R93" s="23"/>
+      <c r="S93" s="23"/>
+      <c r="T93" s="23"/>
+      <c r="U93" s="23"/>
+      <c r="V93" s="23"/>
+      <c r="W93" s="23"/>
+      <c r="X93" s="23"/>
+      <c r="Y93" s="23"/>
+      <c r="Z93" s="23"/>
+      <c r="AA93" s="23"/>
+      <c r="AB93" s="23"/>
+      <c r="AC93" s="23"/>
+      <c r="AD93" s="23"/>
+      <c r="AE93" s="23"/>
+      <c r="AF93" s="23"/>
+      <c r="AG93" s="23"/>
+      <c r="AH93" s="23"/>
+      <c r="AI93" s="23"/>
+    </row>
+    <row r="94" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B94" t="s">
@@ -13790,7 +14388,7 @@
       <c r="C94">
         <v>10084</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="21" t="s">
         <v>372</v>
       </c>
       <c r="E94" t="s">
@@ -13815,9 +14413,33 @@
         <v>43313.690972222219</v>
       </c>
       <c r="L94"/>
-      <c r="M94"/>
-    </row>
-    <row r="95" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M94" s="23"/>
+      <c r="N94" t="s">
+        <v>441</v>
+      </c>
+      <c r="O94" s="23"/>
+      <c r="P94" s="23"/>
+      <c r="Q94" s="23"/>
+      <c r="R94" s="23"/>
+      <c r="S94" s="23"/>
+      <c r="T94" s="23"/>
+      <c r="U94" s="23"/>
+      <c r="V94" s="23"/>
+      <c r="W94" s="23"/>
+      <c r="X94" s="23"/>
+      <c r="Y94" s="23"/>
+      <c r="Z94" s="23"/>
+      <c r="AA94" s="23"/>
+      <c r="AB94" s="23"/>
+      <c r="AC94" s="23"/>
+      <c r="AD94" s="23"/>
+      <c r="AE94" s="23"/>
+      <c r="AF94" s="23"/>
+      <c r="AG94" s="23"/>
+      <c r="AH94" s="23"/>
+      <c r="AI94" s="23"/>
+    </row>
+    <row r="95" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>158</v>
       </c>
@@ -13852,10 +14474,32 @@
         <v>43304.718055555553</v>
       </c>
       <c r="L95"/>
-      <c r="M95"/>
-    </row>
-    <row r="96" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="M95" s="23"/>
+      <c r="N95" s="23"/>
+      <c r="O95" s="23"/>
+      <c r="P95" s="23"/>
+      <c r="Q95" s="23"/>
+      <c r="R95" s="23"/>
+      <c r="S95" s="23"/>
+      <c r="T95" s="23"/>
+      <c r="U95" s="23"/>
+      <c r="V95" s="23"/>
+      <c r="W95" s="23"/>
+      <c r="X95" s="23"/>
+      <c r="Y95" s="23"/>
+      <c r="Z95" s="23"/>
+      <c r="AA95" s="23"/>
+      <c r="AB95" s="23"/>
+      <c r="AC95" s="23"/>
+      <c r="AD95" s="23"/>
+      <c r="AE95" s="23"/>
+      <c r="AF95" s="23"/>
+      <c r="AG95" s="23"/>
+      <c r="AH95" s="23"/>
+      <c r="AI95" s="23"/>
+    </row>
+    <row r="96" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B96" t="s">
@@ -13864,7 +14508,7 @@
       <c r="C96">
         <v>10086</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="21" t="s">
         <v>368</v>
       </c>
       <c r="E96" t="s">
@@ -13889,9 +14533,33 @@
         <v>43304.726388888892</v>
       </c>
       <c r="L96"/>
-      <c r="M96"/>
-    </row>
-    <row r="97" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M96" s="23"/>
+      <c r="N96" t="s">
+        <v>465</v>
+      </c>
+      <c r="O96" s="23"/>
+      <c r="P96" s="23"/>
+      <c r="Q96" s="23"/>
+      <c r="R96" s="23"/>
+      <c r="S96" s="23"/>
+      <c r="T96" s="23"/>
+      <c r="U96" s="23"/>
+      <c r="V96" s="23"/>
+      <c r="W96" s="23"/>
+      <c r="X96" s="23"/>
+      <c r="Y96" s="23"/>
+      <c r="Z96" s="23"/>
+      <c r="AA96" s="23"/>
+      <c r="AB96" s="23"/>
+      <c r="AC96" s="23"/>
+      <c r="AD96" s="23"/>
+      <c r="AE96" s="23"/>
+      <c r="AF96" s="23"/>
+      <c r="AG96" s="23"/>
+      <c r="AH96" s="23"/>
+      <c r="AI96" s="23"/>
+    </row>
+    <row r="97" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>158</v>
       </c>
@@ -13924,10 +14592,34 @@
         <v>43305.89166666667</v>
       </c>
       <c r="L97"/>
-      <c r="M97"/>
-    </row>
-    <row r="98" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="M97" s="23"/>
+      <c r="N97" t="s">
+        <v>466</v>
+      </c>
+      <c r="O97" s="23"/>
+      <c r="P97" s="23"/>
+      <c r="Q97" s="23"/>
+      <c r="R97" s="23"/>
+      <c r="S97" s="23"/>
+      <c r="T97" s="23"/>
+      <c r="U97" s="23"/>
+      <c r="V97" s="23"/>
+      <c r="W97" s="23"/>
+      <c r="X97" s="23"/>
+      <c r="Y97" s="23"/>
+      <c r="Z97" s="23"/>
+      <c r="AA97" s="23"/>
+      <c r="AB97" s="23"/>
+      <c r="AC97" s="23"/>
+      <c r="AD97" s="23"/>
+      <c r="AE97" s="23"/>
+      <c r="AF97" s="23"/>
+      <c r="AG97" s="23"/>
+      <c r="AH97" s="23"/>
+      <c r="AI97" s="23"/>
+    </row>
+    <row r="98" spans="1:35" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B98" t="s">
@@ -13936,7 +14628,7 @@
       <c r="C98">
         <v>10090</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="21" t="s">
         <v>364</v>
       </c>
       <c r="E98" t="s">
@@ -13959,9 +14651,31 @@
         <v>43310.668749999997</v>
       </c>
       <c r="L98"/>
-      <c r="M98"/>
-    </row>
-    <row r="99" spans="1:13" s="10" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M98" s="23"/>
+      <c r="N98" s="23"/>
+      <c r="O98" s="23"/>
+      <c r="P98" s="23"/>
+      <c r="Q98" s="23"/>
+      <c r="R98" s="23"/>
+      <c r="S98" s="23"/>
+      <c r="T98" s="23"/>
+      <c r="U98" s="23"/>
+      <c r="V98" s="23"/>
+      <c r="W98" s="23"/>
+      <c r="X98" s="23"/>
+      <c r="Y98" s="23"/>
+      <c r="Z98" s="23"/>
+      <c r="AA98" s="23"/>
+      <c r="AB98" s="23"/>
+      <c r="AC98" s="23"/>
+      <c r="AD98" s="23"/>
+      <c r="AE98" s="23"/>
+      <c r="AF98" s="23"/>
+      <c r="AG98" s="23"/>
+      <c r="AH98" s="23"/>
+      <c r="AI98" s="23"/>
+    </row>
+    <row r="99" spans="1:35" s="10" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>158</v>
       </c>
@@ -13996,9 +14710,31 @@
         <v>43307.611805555556</v>
       </c>
       <c r="L99"/>
-      <c r="M99"/>
-    </row>
-    <row r="100" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M99" s="23"/>
+      <c r="N99" s="23"/>
+      <c r="O99" s="23"/>
+      <c r="P99" s="23"/>
+      <c r="Q99" s="23"/>
+      <c r="R99" s="23"/>
+      <c r="S99" s="23"/>
+      <c r="T99" s="23"/>
+      <c r="U99" s="23"/>
+      <c r="V99" s="23"/>
+      <c r="W99" s="23"/>
+      <c r="X99" s="23"/>
+      <c r="Y99" s="23"/>
+      <c r="Z99" s="23"/>
+      <c r="AA99" s="23"/>
+      <c r="AB99" s="23"/>
+      <c r="AC99" s="23"/>
+      <c r="AD99" s="23"/>
+      <c r="AE99" s="23"/>
+      <c r="AF99" s="23"/>
+      <c r="AG99" s="23"/>
+      <c r="AH99" s="23"/>
+      <c r="AI99" s="23"/>
+    </row>
+    <row r="100" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="7" t="s">
         <v>4</v>
       </c>
@@ -14011,8 +14747,31 @@
       <c r="H100" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M100" s="23"/>
+      <c r="N100" s="23"/>
+      <c r="O100" s="23"/>
+      <c r="P100" s="23"/>
+      <c r="Q100" s="23"/>
+      <c r="R100" s="23"/>
+      <c r="S100" s="23"/>
+      <c r="T100" s="23"/>
+      <c r="U100" s="23"/>
+      <c r="V100" s="23"/>
+      <c r="W100" s="23"/>
+      <c r="X100" s="23"/>
+      <c r="Y100" s="23"/>
+      <c r="Z100" s="23"/>
+      <c r="AA100" s="23"/>
+      <c r="AB100" s="23"/>
+      <c r="AC100" s="23"/>
+      <c r="AD100" s="23"/>
+      <c r="AE100" s="23"/>
+      <c r="AF100" s="23"/>
+      <c r="AG100" s="23"/>
+      <c r="AH100" s="23"/>
+      <c r="AI100" s="23"/>
+    </row>
+    <row r="101" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="7" t="s">
         <v>6</v>
       </c>
@@ -14025,8 +14784,31 @@
       <c r="H101" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M101" s="23"/>
+      <c r="N101" s="23"/>
+      <c r="O101" s="23"/>
+      <c r="P101" s="23"/>
+      <c r="Q101" s="23"/>
+      <c r="R101" s="23"/>
+      <c r="S101" s="23"/>
+      <c r="T101" s="23"/>
+      <c r="U101" s="23"/>
+      <c r="V101" s="23"/>
+      <c r="W101" s="23"/>
+      <c r="X101" s="23"/>
+      <c r="Y101" s="23"/>
+      <c r="Z101" s="23"/>
+      <c r="AA101" s="23"/>
+      <c r="AB101" s="23"/>
+      <c r="AC101" s="23"/>
+      <c r="AD101" s="23"/>
+      <c r="AE101" s="23"/>
+      <c r="AF101" s="23"/>
+      <c r="AG101" s="23"/>
+      <c r="AH101" s="23"/>
+      <c r="AI101" s="23"/>
+    </row>
+    <row r="102" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="7" t="s">
         <v>6</v>
       </c>
@@ -14039,8 +14821,31 @@
       <c r="H102" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M102" s="23"/>
+      <c r="N102" s="23"/>
+      <c r="O102" s="23"/>
+      <c r="P102" s="23"/>
+      <c r="Q102" s="23"/>
+      <c r="R102" s="23"/>
+      <c r="S102" s="23"/>
+      <c r="T102" s="23"/>
+      <c r="U102" s="23"/>
+      <c r="V102" s="23"/>
+      <c r="W102" s="23"/>
+      <c r="X102" s="23"/>
+      <c r="Y102" s="23"/>
+      <c r="Z102" s="23"/>
+      <c r="AA102" s="23"/>
+      <c r="AB102" s="23"/>
+      <c r="AC102" s="23"/>
+      <c r="AD102" s="23"/>
+      <c r="AE102" s="23"/>
+      <c r="AF102" s="23"/>
+      <c r="AG102" s="23"/>
+      <c r="AH102" s="23"/>
+      <c r="AI102" s="23"/>
+    </row>
+    <row r="103" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="7" t="s">
         <v>6</v>
       </c>
@@ -14053,8 +14858,31 @@
       <c r="H103" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M103" s="23"/>
+      <c r="N103" s="23"/>
+      <c r="O103" s="23"/>
+      <c r="P103" s="23"/>
+      <c r="Q103" s="23"/>
+      <c r="R103" s="23"/>
+      <c r="S103" s="23"/>
+      <c r="T103" s="23"/>
+      <c r="U103" s="23"/>
+      <c r="V103" s="23"/>
+      <c r="W103" s="23"/>
+      <c r="X103" s="23"/>
+      <c r="Y103" s="23"/>
+      <c r="Z103" s="23"/>
+      <c r="AA103" s="23"/>
+      <c r="AB103" s="23"/>
+      <c r="AC103" s="23"/>
+      <c r="AD103" s="23"/>
+      <c r="AE103" s="23"/>
+      <c r="AF103" s="23"/>
+      <c r="AG103" s="23"/>
+      <c r="AH103" s="23"/>
+      <c r="AI103" s="23"/>
+    </row>
+    <row r="104" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="8" t="s">
         <v>217</v>
       </c>
@@ -14068,7 +14896,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="7" t="s">
         <v>6</v>
       </c>
@@ -14082,7 +14910,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="7" t="s">
         <v>11</v>
       </c>
@@ -14096,7 +14924,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="8" t="s">
         <v>217</v>
       </c>
@@ -14110,7 +14938,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="7" t="s">
         <v>4</v>
       </c>
@@ -14124,7 +14952,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="7" t="s">
         <v>15</v>
       </c>
@@ -14138,7 +14966,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
         <v>4</v>
       </c>
@@ -14152,7 +14980,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="7" t="s">
         <v>218</v>
       </c>
@@ -14166,7 +14994,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:35" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="7" t="s">
         <v>218</v>
       </c>
@@ -14215,10 +15043,11 @@
       <c r="D115" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="F115" s="21"/>
       <c r="G115" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H115" t="s">
+      <c r="H115" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14229,10 +15058,11 @@
       <c r="D116" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="F116" s="21"/>
       <c r="G116" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H116" t="s">
+      <c r="H116" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14243,10 +15073,11 @@
       <c r="D117" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="F117" s="21"/>
       <c r="G117" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H117" t="s">
+      <c r="H117" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14327,10 +15158,11 @@
       <c r="D123" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="F123" s="21"/>
       <c r="G123" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H123" t="s">
+      <c r="H123" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14341,10 +15173,11 @@
       <c r="D124" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="F124" s="21"/>
       <c r="G124" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H124" t="s">
+      <c r="H124" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14355,10 +15188,11 @@
       <c r="D125" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="F125" s="21"/>
       <c r="G125" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H125" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14369,10 +15203,11 @@
       <c r="D126" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="F126" s="21"/>
       <c r="G126" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H126" t="s">
+      <c r="H126" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14383,10 +15218,11 @@
       <c r="D127" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F127" s="21"/>
       <c r="G127" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H127" t="s">
+      <c r="H127" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14411,10 +15247,11 @@
       <c r="D129" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="F129" s="21"/>
       <c r="G129" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H129" t="s">
+      <c r="H129" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14439,10 +15276,11 @@
       <c r="D131" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="F131" s="21"/>
       <c r="G131" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H131" t="s">
+      <c r="H131" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14481,10 +15319,11 @@
       <c r="D134" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="F134" s="21"/>
       <c r="G134" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H134" t="s">
+      <c r="H134" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14495,10 +15334,11 @@
       <c r="D135" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="F135" s="21"/>
       <c r="G135" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H135" t="s">
+      <c r="H135" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14509,10 +15349,11 @@
       <c r="D136" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="F136" s="21"/>
       <c r="G136" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H136" t="s">
+      <c r="H136" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14523,10 +15364,11 @@
       <c r="D137" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="F137" s="21"/>
       <c r="G137" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H137" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14596,7 +15438,7 @@
       <c r="G142" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H142" t="s">
+      <c r="H142" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14624,7 +15466,7 @@
       <c r="G144" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H144" t="s">
+      <c r="H144" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14638,7 +15480,7 @@
       <c r="G145" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H145" t="s">
+      <c r="H145" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14694,7 +15536,7 @@
       <c r="G149" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H149" t="s">
+      <c r="H149" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14708,7 +15550,7 @@
       <c r="G150" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H150" t="s">
+      <c r="H150" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14722,7 +15564,7 @@
       <c r="G151" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H151" t="s">
+      <c r="H151" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14806,7 +15648,7 @@
       <c r="G157" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H157" t="s">
+      <c r="H157" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14834,7 +15676,7 @@
       <c r="G159" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H159" t="s">
+      <c r="H159" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14876,7 +15718,7 @@
       <c r="G162" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H162" t="s">
+      <c r="H162" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14890,7 +15732,7 @@
       <c r="G163" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H163" t="s">
+      <c r="H163" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -14904,7 +15746,7 @@
       <c r="G164" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H164" t="s">
+      <c r="H164" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15002,7 +15844,7 @@
       <c r="G171" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H171" t="s">
+      <c r="H171" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15030,7 +15872,7 @@
       <c r="G173" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H173" t="s">
+      <c r="H173" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15058,7 +15900,7 @@
       <c r="G175" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H175" t="s">
+      <c r="H175" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15072,7 +15914,7 @@
       <c r="G176" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H176" t="s">
+      <c r="H176" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15408,7 +16250,7 @@
       <c r="G200" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H200" t="s">
+      <c r="H200" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15450,7 +16292,7 @@
       <c r="G203" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H203" t="s">
+      <c r="H203" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15478,7 +16320,7 @@
       <c r="G205" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H205" t="s">
+      <c r="H205" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15492,7 +16334,7 @@
       <c r="G206" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="H206" t="s">
+      <c r="H206" s="21" t="s">
         <v>399</v>
       </c>
     </row>
@@ -15539,7 +16381,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M209"/>
+  <autoFilter ref="A1:AI1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>